<commit_message>
fixed shuffling; added 9 restaurants & food types
</commit_message>
<xml_diff>
--- a/psychopy-2/runs.xlsx
+++ b/psychopy-2/runs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="6940" windowWidth="19960" windowHeight="10520" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="9840" windowWidth="19960" windowHeight="10520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>restaurantNames</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Le Parisien,Chez Toinette,Au Petit Sud Ouest</t>
   </si>
   <si>
-    <t>Lau's Dim Sum Bar,OO Kook Korean BBQ,Happy Lamb Hot Pot</t>
-  </si>
-  <si>
-    <t>asian_food</t>
-  </si>
-  <si>
     <t>french_food</t>
   </si>
   <si>
@@ -58,13 +52,55 @@
   </si>
   <si>
     <t>Okay here's how this works. Each row is a different run -- a list of restaurant names + the prefix of the filenames of its corresponding foods. The list of restaurant names should be comma-separated and should contain exactly 3 restaurants (no unicode characters please -- stick to ASCII). For each food prefix, there should be 3 corresponding files in the 'foods' directory in the format "[food prefix][cueId].png". For example, for the prefix "mexican_food", there should be files "mexican_food0.png", "mexican_food1.png" and "mexican_food2.png".  The third column is randomly shuffled so different foods/restaurants can be used with different context roles across subjects. The context role also corresponds to the filename where the context/cue pairs are, in the format "[contextRole].xlsx". In each of these files, the contextId and cueId are matched with the restaurants and foods, respectively. Sorry it's so complicated but there is no other way to make it work with psychopy</t>
+  </si>
+  <si>
+    <t>chinese_food</t>
+  </si>
+  <si>
+    <t>Breakfast at Tiffany's,Sweet Maple,Mission Beach Cafe</t>
+  </si>
+  <si>
+    <t>brunch_food</t>
+  </si>
+  <si>
+    <t>greek_food</t>
+  </si>
+  <si>
+    <t>Myconos Restaurant,Mediterranean Grill,Gyro King</t>
+  </si>
+  <si>
+    <t>japanese_food</t>
+  </si>
+  <si>
+    <t>sushi_food</t>
+  </si>
+  <si>
+    <t>Lau's Dim Sum Bar,Shanghai Dumpling King,Happy Lamb Hot Pot</t>
+  </si>
+  <si>
+    <t>Izakaya Sozai,Onigilly Express,Sanraku Restaurant</t>
+  </si>
+  <si>
+    <t>Kusakabe,Sara Sushi Bar,Wako Sushi Place</t>
+  </si>
+  <si>
+    <t>italian_food</t>
+  </si>
+  <si>
+    <t>Restorante Milano,Trattoria Contadina,Fino Bar &amp; Restorante</t>
+  </si>
+  <si>
+    <t>fast_food</t>
+  </si>
+  <si>
+    <t>McRonald's,Burger Queen,Metro Drive-In</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,6 +131,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -113,8 +165,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -126,7 +180,9 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,15 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="1" max="1" width="65.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -476,25 +532,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -502,21 +558,87 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -524,6 +646,7 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
inidan foods, rm sushi, full random test trials
end trial on key press => undo
</commit_message>
<xml_diff>
--- a/psychopy-2/runs.xlsx
+++ b/psychopy-2/runs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="9840" windowWidth="19960" windowHeight="10520" tabRatio="500"/>
+    <workbookView xWindow="-4240" yWindow="-23540" windowWidth="21840" windowHeight="11880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,18 +72,12 @@
     <t>japanese_food</t>
   </si>
   <si>
-    <t>sushi_food</t>
-  </si>
-  <si>
     <t>Lau's Dim Sum Bar,Shanghai Dumpling King,Happy Lamb Hot Pot</t>
   </si>
   <si>
     <t>Izakaya Sozai,Onigilly Express,Sanraku Restaurant</t>
   </si>
   <si>
-    <t>Kusakabe,Sara Sushi Bar,Wako Sushi Place</t>
-  </si>
-  <si>
     <t>italian_food</t>
   </si>
   <si>
@@ -93,7 +87,13 @@
     <t>fast_food</t>
   </si>
   <si>
-    <t>McRonald's,Burger Queen,Metro Drive-In</t>
+    <t>Dave's Sandwiches,Burger Masters,Metro Drive-In</t>
+  </si>
+  <si>
+    <t>indian_food</t>
+  </si>
+  <si>
+    <t>Little Delhi House,Curry Leaf Restaurant,Tandoori Kitchen</t>
   </si>
 </sst>
 </file>
@@ -515,13 +515,14 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="65.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -566,7 +567,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -599,7 +600,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -610,10 +611,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -621,10 +622,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -632,10 +633,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>

</xml_diff>